<commit_message>
Added in Druid skills doc 5 new skills.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/Done/5-Elementalist/Documentation/ElementalistSkills.xlsx
+++ b/GameDesign/Class/Done/5-Elementalist/Documentation/ElementalistSkills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="5" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="1-Pillar" sheetId="1" r:id="rId1"/>
@@ -842,7 +842,7 @@
   <dimension ref="B2:D46"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1133,7 +1133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D30"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
@@ -1330,7 +1330,7 @@
   <dimension ref="B2:D25"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1977,7 +1977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>

</xml_diff>